<commit_message>
Update JacobiDataSource to support formula as matrix dimension
</commit_message>
<xml_diff>
--- a/jacobi/src/test/resources/jacobi/test/data/JacobiJUnit4ClassRunnerTest.xlsx
+++ b/jacobi/src/test/resources/jacobi/test/data/JacobiJUnit4ClassRunnerTest.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="testReadEquals3x3" sheetId="1" r:id="rId1"/>
     <sheet name="testReadEquals5x5" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="test Dynamic Dimension 1x7" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>#1</t>
   </si>
@@ -574,7 +574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -816,12 +816,53 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>COUNTA(A3:A8)</f>
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f>COUNTA(3:3)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>